<commit_message>
docs: Documentación final final
</commit_message>
<xml_diff>
--- a/docs/basesDatos/Documentacion_base_de_datos.xlsx
+++ b/docs/basesDatos/Documentacion_base_de_datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php\proyecto_aula\ProyectoAula\docs\basesDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E75A7-B06D-41E6-8540-1923C2F2817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF97858-ECD3-4717-8FF3-161E8D8FDED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C55D8C36-47C5-4AF1-979D-52B52F76DB07}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="234">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -155,9 +155,6 @@
     <t>FK</t>
   </si>
   <si>
-    <t>ID del usuario, no es su número de cuenta y contiene autoincrement</t>
-  </si>
-  <si>
     <t>Nombre(s) del usuario, sin apellidos</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>tipo_usuario</t>
   </si>
   <si>
-    <t>ID que numera los tipos de usuario, existen 4, por lo que hay 4 IDs.</t>
-  </si>
-  <si>
     <t>Nombre que describe a los tipos de usuario, ejemplo: estudiante.</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>text(max)</t>
   </si>
   <si>
-    <t>ID de la duda, contiene autoincrement</t>
-  </si>
-  <si>
     <t>Descripción de la duda, la duda que expresará el usuario en el foro</t>
   </si>
   <si>
@@ -242,9 +233,6 @@
     <t>Imagen con la que el usuario se identifica, funge de avatar, no es obligatorio</t>
   </si>
   <si>
-    <t>ID que relaciona un número autoincrement con la respuesta de un usuario a una duda de otro usuario</t>
-  </si>
-  <si>
     <t>Es la respuesta que brinda un usuario a una duda del foro</t>
   </si>
   <si>
@@ -266,9 +254,6 @@
     <t>ID_evento</t>
   </si>
   <si>
-    <t>ID de una tabla has, por lo que sólo existen 2 IDs, los de sus llaves foráneas</t>
-  </si>
-  <si>
     <t>Llave foránea que nos lleva a la tabla usuario, pues no todos los usuarios tienen los mismos eventos</t>
   </si>
   <si>
@@ -290,9 +275,6 @@
     <t>varchar(300)</t>
   </si>
   <si>
-    <t>ID que relaciona un número autoincrement con un evento específico</t>
-  </si>
-  <si>
     <t>Llave foránea que nos lleva a la tabla tipoevento, donde podremos identificar si se trata de un evento social o académico</t>
   </si>
   <si>
@@ -461,9 +443,6 @@
     <t>ruta_archivos</t>
   </si>
   <si>
-    <t>texto_tarea</t>
-  </si>
-  <si>
     <t>ID_entrega</t>
   </si>
   <si>
@@ -488,9 +467,6 @@
     <t>Se puede agregar una imagen a la actividad relacionada con ella</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Fecha en la que la actividad se publicó</t>
   </si>
   <si>
@@ -512,9 +488,6 @@
     <t>calif</t>
   </si>
   <si>
-    <t>ruta_links</t>
-  </si>
-  <si>
     <t>fecha_entr</t>
   </si>
   <si>
@@ -563,9 +536,6 @@
     <t>Llave foránea que relaciona la tabla juego con la tabla preguntas, pues los juegos están compuestos de preguntas que el usuario deberá contestar correctamente</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>preguntas</t>
   </si>
   <si>
@@ -716,10 +686,58 @@
     <t>Se puede guardar la ruta de un archivo para que se despliegue en el tablón</t>
   </si>
   <si>
-    <t>Llave foránea que relaciona la tabla archivosTablon</t>
-  </si>
-  <si>
     <t>Relaciona un número que identifica los registros de la tabla archivostablon</t>
+  </si>
+  <si>
+    <t>coment_profe</t>
+  </si>
+  <si>
+    <t>coment_alumno</t>
+  </si>
+  <si>
+    <t>Verificador que indica si la respuesta es o no es correcta, cuando es correcta toma el número 1 y cuando es incorreta toma el 0</t>
+  </si>
+  <si>
+    <t>Se tiene la opción de que el profesor pueda agregar comentarios a la actividad del usuario</t>
+  </si>
+  <si>
+    <t>Se tiene la opción de que el usuario pueda agregar comentarios a la retroalimentación del profesor</t>
+  </si>
+  <si>
+    <t>ulikesmaterial</t>
+  </si>
+  <si>
+    <t>ID_ULikesMaterial</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla ulikesmaterial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llave foránea que relaciona la tabla archivosTablon con la tabla material </t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla tipousuario</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla usuario</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla duda</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla dudaresp</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla usuariohasevento</t>
+  </si>
+  <si>
+    <t>Relaciona un número que identifica los registros de la tabla evento</t>
+  </si>
+  <si>
+    <t>Llave foránea que relaciona la tabla ulikesmaterial con la tabla usuario, pues queremos saber qué usuario es el que le ha dado like al material</t>
+  </si>
+  <si>
+    <t>Llave foránea que relaciona la tabla ulikesmaterial con la tabla material, ya que queremos saber a qué material le ha dado like el usuario</t>
   </si>
 </sst>
 </file>
@@ -1074,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F299159E-CF19-45D0-9A7D-570B3394ADE5}">
   <dimension ref="B1:L111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="L109" sqref="L109"/>
+    <sheetView tabSelected="1" topLeftCell="B90" workbookViewId="0">
+      <selection activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1161,7 @@
         <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -1163,7 +1181,7 @@
         <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -1183,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1206,7 +1224,7 @@
         <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -1226,7 +1244,7 @@
         <v>34</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -1249,7 +1267,7 @@
         <v>37</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -1269,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="L8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -1292,7 +1310,7 @@
         <v>37</v>
       </c>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -1315,7 +1333,7 @@
         <v>38</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -1335,7 +1353,7 @@
         <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -1358,7 +1376,7 @@
         <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -1378,12 +1396,12 @@
         <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1401,15 +1419,15 @@
         <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>51</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1424,15 +1442,15 @@
         <v>37</v>
       </c>
       <c r="L15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -1447,52 +1465,52 @@
         <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="E17" t="s">
-        <v>59</v>
-      </c>
       <c r="F17" t="s">
         <v>34</v>
       </c>
       <c r="L17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
       </c>
       <c r="L18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1510,15 +1528,15 @@
         <v>38</v>
       </c>
       <c r="L19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
@@ -1533,52 +1551,52 @@
         <v>36</v>
       </c>
       <c r="L20" t="s">
-        <v>68</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
         <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" t="s">
-        <v>58</v>
-      </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1596,15 +1614,15 @@
         <v>38</v>
       </c>
       <c r="L23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
@@ -1619,15 +1637,15 @@
         <v>38</v>
       </c>
       <c r="L24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
@@ -1642,15 +1660,15 @@
         <v>36</v>
       </c>
       <c r="L25" t="s">
-        <v>76</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
         <v>23</v>
@@ -1665,12 +1683,12 @@
         <v>38</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1688,15 +1706,15 @@
         <v>38</v>
       </c>
       <c r="L27" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
@@ -1711,15 +1729,15 @@
         <v>36</v>
       </c>
       <c r="L28" t="s">
-        <v>84</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
@@ -1734,75 +1752,75 @@
         <v>38</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
       <c r="L30" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
         <v>55</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>57</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
       </c>
       <c r="L31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
         <v>35</v>
       </c>
       <c r="L32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
@@ -1817,12 +1835,12 @@
         <v>36</v>
       </c>
       <c r="L33" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -1831,7 +1849,7 @@
         <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -1840,15 +1858,15 @@
         <v>37</v>
       </c>
       <c r="L34" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
@@ -1863,12 +1881,12 @@
         <v>36</v>
       </c>
       <c r="L35" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1886,15 +1904,15 @@
         <v>38</v>
       </c>
       <c r="L36" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
@@ -1909,15 +1927,15 @@
         <v>38</v>
       </c>
       <c r="L37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
         <v>23</v>
@@ -1932,35 +1950,35 @@
         <v>36</v>
       </c>
       <c r="L38" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
         <v>24</v>
       </c>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
       </c>
       <c r="L39" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
         <v>23</v>
@@ -1972,15 +1990,15 @@
         <v>35</v>
       </c>
       <c r="L40" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>23</v>
@@ -1995,15 +2013,15 @@
         <v>36</v>
       </c>
       <c r="L41" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
         <v>23</v>
@@ -2018,15 +2036,15 @@
         <v>38</v>
       </c>
       <c r="L42" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
         <v>23</v>
@@ -2041,15 +2059,15 @@
         <v>38</v>
       </c>
       <c r="L43" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
         <v>23</v>
@@ -2064,15 +2082,15 @@
         <v>36</v>
       </c>
       <c r="L44" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
         <v>24</v>
@@ -2087,32 +2105,32 @@
         <v>37</v>
       </c>
       <c r="L45" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
         <v>25</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L46" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -2127,15 +2145,15 @@
         <v>35</v>
       </c>
       <c r="L47" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
         <v>23</v>
@@ -2150,12 +2168,12 @@
         <v>36</v>
       </c>
       <c r="L48" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
@@ -2173,15 +2191,15 @@
         <v>38</v>
       </c>
       <c r="L49" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
         <v>23</v>
@@ -2196,15 +2214,15 @@
         <v>38</v>
       </c>
       <c r="L50" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
         <v>23</v>
@@ -2219,12 +2237,12 @@
         <v>36</v>
       </c>
       <c r="L51" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C52" t="s">
         <v>12</v>
@@ -2242,15 +2260,15 @@
         <v>38</v>
       </c>
       <c r="L52" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
         <v>23</v>
@@ -2265,15 +2283,15 @@
         <v>38</v>
       </c>
       <c r="L53" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D54" t="s">
         <v>23</v>
@@ -2288,15 +2306,15 @@
         <v>36</v>
       </c>
       <c r="L54" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
         <v>23</v>
@@ -2311,15 +2329,15 @@
         <v>38</v>
       </c>
       <c r="L55" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
         <v>23</v>
@@ -2334,15 +2352,15 @@
         <v>38</v>
       </c>
       <c r="L56" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s">
         <v>23</v>
@@ -2357,12 +2375,12 @@
         <v>36</v>
       </c>
       <c r="L57" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
         <v>13</v>
@@ -2377,15 +2395,15 @@
         <v>34</v>
       </c>
       <c r="L58" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D59" t="s">
         <v>23</v>
@@ -2400,15 +2418,15 @@
         <v>36</v>
       </c>
       <c r="L59" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
         <v>24</v>
@@ -2420,12 +2438,12 @@
         <v>34</v>
       </c>
       <c r="L60" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C61" t="s">
         <v>13</v>
@@ -2440,95 +2458,98 @@
         <v>34</v>
       </c>
       <c r="L61" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>34</v>
       </c>
       <c r="L62" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D63" t="s">
         <v>25</v>
       </c>
       <c r="E63" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F63" t="s">
         <v>35</v>
       </c>
       <c r="L63" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>54</v>
       </c>
       <c r="D64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E64" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="F64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L64" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="E65" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="F65" t="s">
         <v>34</v>
       </c>
+      <c r="I65" t="s">
+        <v>38</v>
+      </c>
       <c r="L65" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
         <v>23</v>
@@ -2543,58 +2564,58 @@
         <v>38</v>
       </c>
       <c r="L66" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" t="s">
         <v>136</v>
       </c>
-      <c r="C67" t="s">
-        <v>142</v>
-      </c>
       <c r="D67" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E67" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="F67" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L67" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C68" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E68" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="F68" t="s">
         <v>35</v>
       </c>
+      <c r="I68" t="s">
+        <v>38</v>
+      </c>
       <c r="L68" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D69" t="s">
         <v>23</v>
@@ -2603,181 +2624,193 @@
         <v>23</v>
       </c>
       <c r="F69" t="s">
-        <v>35</v>
-      </c>
-      <c r="I69" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="H69" t="s">
+        <v>36</v>
       </c>
       <c r="L69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" t="s">
+        <v>23</v>
+      </c>
+      <c r="F70" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" t="s">
+        <v>38</v>
+      </c>
+      <c r="L70" t="s">
         <v>155</v>
-      </c>
-      <c r="C70" t="s">
-        <v>156</v>
-      </c>
-      <c r="D70" t="s">
-        <v>23</v>
-      </c>
-      <c r="E70" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" t="s">
-        <v>34</v>
-      </c>
-      <c r="H70" t="s">
-        <v>36</v>
-      </c>
-      <c r="L70" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="F71" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L71" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="E72" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="F72" t="s">
         <v>35</v>
       </c>
       <c r="L72" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="D73" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E73" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="F73" t="s">
         <v>35</v>
       </c>
+      <c r="L73" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E74" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="L74" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E75" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="F75" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I75" t="s">
+        <v>38</v>
+      </c>
+      <c r="L75" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D76" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="E76" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="F76" t="s">
         <v>34</v>
       </c>
+      <c r="H76" t="s">
+        <v>36</v>
+      </c>
       <c r="L76" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E77" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="F77" t="s">
         <v>34</v>
       </c>
-      <c r="I77" t="s">
-        <v>38</v>
+      <c r="J77" t="s">
+        <v>37</v>
       </c>
       <c r="L77" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D78" t="s">
         <v>23</v>
@@ -2792,38 +2825,38 @@
         <v>36</v>
       </c>
       <c r="L78" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="D79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E79" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="F79" t="s">
         <v>34</v>
       </c>
-      <c r="J79" t="s">
-        <v>37</v>
+      <c r="I79" t="s">
+        <v>38</v>
       </c>
       <c r="L79" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C80" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
         <v>23</v>
@@ -2838,55 +2871,52 @@
         <v>36</v>
       </c>
       <c r="L80" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C81" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D81" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E81" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="F81" t="s">
         <v>34</v>
       </c>
-      <c r="I81" t="s">
-        <v>38</v>
-      </c>
       <c r="L81" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C82" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D82" t="s">
         <v>25</v>
       </c>
       <c r="E82" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F82" t="s">
         <v>35</v>
       </c>
       <c r="L82" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C83" t="s">
         <v>172</v>
@@ -2904,78 +2934,78 @@
         <v>36</v>
       </c>
       <c r="L83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C84" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" t="s">
+        <v>23</v>
+      </c>
+      <c r="E84" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" t="s">
+        <v>34</v>
+      </c>
+      <c r="I84" t="s">
+        <v>38</v>
+      </c>
+      <c r="L84" t="s">
         <v>177</v>
-      </c>
-      <c r="D84" t="s">
-        <v>57</v>
-      </c>
-      <c r="E84" t="s">
-        <v>145</v>
-      </c>
-      <c r="F84" t="s">
-        <v>34</v>
-      </c>
-      <c r="L84" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C85" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="D85" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E85" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
       <c r="F85" t="s">
         <v>35</v>
       </c>
       <c r="L85" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D86" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E86" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="F86" t="s">
-        <v>34</v>
-      </c>
-      <c r="H86" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L86" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C87" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D87" t="s">
         <v>23</v>
@@ -2986,56 +3016,62 @@
       <c r="F87" t="s">
         <v>34</v>
       </c>
-      <c r="I87" t="s">
-        <v>38</v>
+      <c r="H87" t="s">
+        <v>36</v>
       </c>
       <c r="L87" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" t="s">
         <v>181</v>
       </c>
-      <c r="C88" t="s">
-        <v>183</v>
-      </c>
       <c r="D88" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E88" t="s">
-        <v>185</v>
+        <v>78</v>
       </c>
       <c r="F88" t="s">
         <v>35</v>
       </c>
+      <c r="L88" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C89" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="D89" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E89" t="s">
-        <v>145</v>
+        <v>23</v>
       </c>
       <c r="F89" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I89" t="s">
+        <v>38</v>
       </c>
       <c r="L89" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C90" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D90" t="s">
         <v>23</v>
@@ -3046,59 +3082,59 @@
       <c r="F90" t="s">
         <v>34</v>
       </c>
-      <c r="H90" t="s">
-        <v>36</v>
+      <c r="I90" t="s">
+        <v>38</v>
       </c>
       <c r="L90" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>187</v>
+      </c>
+      <c r="C91" t="s">
+        <v>188</v>
+      </c>
+      <c r="D91" t="s">
+        <v>23</v>
+      </c>
+      <c r="E91" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" t="s">
+        <v>34</v>
+      </c>
+      <c r="H91" t="s">
+        <v>36</v>
+      </c>
+      <c r="L91" t="s">
         <v>189</v>
-      </c>
-      <c r="C91" t="s">
-        <v>191</v>
-      </c>
-      <c r="D91" t="s">
-        <v>25</v>
-      </c>
-      <c r="E91" t="s">
-        <v>83</v>
-      </c>
-      <c r="F91" t="s">
-        <v>35</v>
-      </c>
-      <c r="L91" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="D92" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E92" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F92" t="s">
         <v>34</v>
       </c>
-      <c r="I92" t="s">
-        <v>38</v>
-      </c>
       <c r="L92" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C93" t="s">
         <v>192</v>
@@ -3112,62 +3148,62 @@
       <c r="F93" t="s">
         <v>34</v>
       </c>
-      <c r="I93" t="s">
-        <v>38</v>
+      <c r="H93" t="s">
+        <v>36</v>
       </c>
       <c r="L93" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C94" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="D94" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E94" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F94" t="s">
-        <v>34</v>
-      </c>
-      <c r="H94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L94" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="D95" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E95" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F95" t="s">
         <v>34</v>
       </c>
+      <c r="I95" t="s">
+        <v>38</v>
+      </c>
       <c r="L95" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C96" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="D96" t="s">
         <v>23</v>
@@ -3178,28 +3214,31 @@
       <c r="F96" t="s">
         <v>34</v>
       </c>
-      <c r="H96" t="s">
-        <v>36</v>
+      <c r="I96" t="s">
+        <v>38</v>
       </c>
       <c r="L96" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C97" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D97" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E97" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F97" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H97" t="s">
+        <v>36</v>
       </c>
       <c r="L97" t="s">
         <v>204</v>
@@ -3207,10 +3246,10 @@
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C98" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="D98" t="s">
         <v>23</v>
@@ -3230,10 +3269,10 @@
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C99" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D99" t="s">
         <v>23</v>
@@ -3242,10 +3281,7 @@
         <v>23</v>
       </c>
       <c r="F99" t="s">
-        <v>34</v>
-      </c>
-      <c r="I99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L99" t="s">
         <v>206</v>
@@ -3253,33 +3289,33 @@
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
+        <v>197</v>
+      </c>
+      <c r="C100" t="s">
+        <v>200</v>
+      </c>
+      <c r="D100" t="s">
+        <v>23</v>
+      </c>
+      <c r="E100" t="s">
+        <v>23</v>
+      </c>
+      <c r="F100" t="s">
+        <v>34</v>
+      </c>
+      <c r="I100" t="s">
+        <v>38</v>
+      </c>
+      <c r="L100" t="s">
         <v>207</v>
-      </c>
-      <c r="C100" t="s">
-        <v>208</v>
-      </c>
-      <c r="D100" t="s">
-        <v>23</v>
-      </c>
-      <c r="E100" t="s">
-        <v>23</v>
-      </c>
-      <c r="F100" t="s">
-        <v>34</v>
-      </c>
-      <c r="H100" t="s">
-        <v>36</v>
-      </c>
-      <c r="L100" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C101" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="D101" t="s">
         <v>23</v>
@@ -3294,58 +3330,55 @@
         <v>38</v>
       </c>
       <c r="L101" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C102" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D102" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E102" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="F102" t="s">
         <v>35</v>
       </c>
       <c r="L102" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C103" t="s">
+        <v>201</v>
+      </c>
+      <c r="D103" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" t="s">
+        <v>30</v>
+      </c>
+      <c r="F103" t="s">
+        <v>35</v>
+      </c>
+      <c r="L103" t="s">
         <v>210</v>
-      </c>
-      <c r="D103" t="s">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s">
-        <v>23</v>
-      </c>
-      <c r="F103" t="s">
-        <v>34</v>
-      </c>
-      <c r="I103" t="s">
-        <v>38</v>
-      </c>
-      <c r="L103" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C104" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="D104" t="s">
         <v>23</v>
@@ -3354,101 +3387,104 @@
         <v>23</v>
       </c>
       <c r="F104" t="s">
-        <v>34</v>
-      </c>
-      <c r="I104" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L104" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C105" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
       <c r="D105" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E105" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F105" t="s">
         <v>35</v>
       </c>
       <c r="L105" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D106" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E106" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F106" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H106" t="s">
+        <v>36</v>
       </c>
       <c r="L106" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C107" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="D107" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E107" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F107" t="s">
         <v>35</v>
       </c>
       <c r="L107" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C108" t="s">
-        <v>81</v>
+        <v>198</v>
       </c>
       <c r="D108" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="E108" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="F108" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I108" t="s">
+        <v>38</v>
       </c>
       <c r="L108" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>222</v>
+      </c>
+      <c r="C109" t="s">
         <v>223</v>
-      </c>
-      <c r="C109" t="s">
-        <v>224</v>
       </c>
       <c r="D109" t="s">
         <v>23</v>
@@ -3463,35 +3499,38 @@
         <v>36</v>
       </c>
       <c r="L109" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C110" t="s">
-        <v>191</v>
+        <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E110" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F110" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I110" t="s">
+        <v>38</v>
       </c>
       <c r="L110" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C111" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D111" t="s">
         <v>23</v>
@@ -3506,7 +3545,7 @@
         <v>38</v>
       </c>
       <c r="L111" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>